<commit_message>
Use HSQLDB for JDBC-related tests, instead of mocking up own classes.  Modified site's 0.6.0 release date.
</commit_message>
<xml_diff>
--- a/jett-core/templates/JDBCExecutorTemplate.xlsx
+++ b/jett-core/templates/JDBCExecutorTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22035" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="22035" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Query" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
-    <t>${employee.lastName}</t>
-  </si>
-  <si>
     <t>${employee.salary}</t>
   </si>
   <si>
@@ -50,22 +47,25 @@
     <t>${employee.manager}</t>
   </si>
   <si>
-    <t>${employee.catchPhrase}</t>
-  </si>
-  <si>
-    <t>${employee.aManager}&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
-    <t>&lt;jt:forEach items="${jdbc.execQuery('SELECT * FROM employee')}" var="employee" &gt;${employee.firstName}</t>
-  </si>
-  <si>
-    <t>&lt;jt:forEach items="${jdbc.execQuery('SELECT * FROM employee WHERE title = ?', titleSearch)}" var="employee" &gt;${employee.firstName}</t>
-  </si>
-  <si>
     <t>&lt;jt:forEach items="${titleSearches}" var="titleSearch"&gt;${titleSearch}</t>
   </si>
   <si>
-    <t>${employee.aManager}&lt;/jt:forEach&gt;&lt;/jt:forEach&gt;</t>
+    <t>&lt;jt:forEach items="${jdbc.execQuery('SELECT * FROM employee WHERE title = ?', titleSearch)}" var="employee" &gt;${employee.first_name}</t>
+  </si>
+  <si>
+    <t>${employee.last_name}</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${jdbc.execQuery('SELECT * FROM employee')}" var="employee" &gt;${employee.first_name}</t>
+  </si>
+  <si>
+    <t>${employee.catch_phrase}</t>
+  </si>
+  <si>
+    <t>${employee.is_a_manager}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${employee.is_a_manager}&lt;/jt:forEach&gt;&lt;/jt:forEach&gt;</t>
   </si>
 </sst>
 </file>
@@ -477,9 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -491,25 +489,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -517,22 +515,22 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -545,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
@@ -559,7 +557,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -570,45 +568,45 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Ticket 38 - Check for null values in the ResultSet when storing values in the ResultSetRow in JDBCExecutor.
</commit_message>
<xml_diff>
--- a/jett-core/templates/JDBCExecutorTemplate.xlsx
+++ b/jett-core/templates/JDBCExecutorTemplate.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22035" windowHeight="11310"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="22035" windowHeight="11310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Query" sheetId="1" r:id="rId1"/>
     <sheet name="Prepared" sheetId="2" r:id="rId2"/>
+    <sheet name="LessGreater" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>${employee.salary}</t>
   </si>
@@ -66,6 +67,9 @@
   </si>
   <si>
     <t>${employee.is_a_manager}&lt;/jt:forEach&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:forEach items="${jdbc.execQuery('SELECT * FROM employee WHERE first_name &lt;&gt; \\'Randy\\'')}" var="employee" &gt;${employee.first_name}</t>
   </si>
 </sst>
 </file>
@@ -477,7 +481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -544,7 +550,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,4 +624,69 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ticket 41 - When performing escape replacement, replace all instances.  When replacing expressions with values, continue replacing them only one at a time.
</commit_message>
<xml_diff>
--- a/jett-core/templates/JDBCExecutorTemplate.xlsx
+++ b/jett-core/templates/JDBCExecutorTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22035" windowHeight="11310" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="22035" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Query" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,9 @@
     <t>${employee.is_a_manager}&lt;/jt:forEach&gt;&lt;/jt:forEach&gt;</t>
   </si>
   <si>
-    <t>&lt;jt:forEach items="${jdbc.execQuery('SELECT * FROM employee WHERE first_name &lt;&gt; \\'Randy\\'')}" var="employee" &gt;${employee.first_name}</t>
+    <t>&lt;jt:forEach items="${jdbc.execQuery('SELECT *
+FROM employee
+WHERE first_name &lt;&gt; \\'Randy\\'')}" var="employee" &gt;${employee.first_name}</t>
   </si>
 </sst>
 </file>
@@ -157,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -173,6 +175,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,9 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -550,7 +551,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -664,7 +665,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">

</xml_diff>